<commit_message>
docs: Fixed a copy/paste error in the assignment documentation (table)
</commit_message>
<xml_diff>
--- a/docs/codegen_cases_assign.xlsx
+++ b/docs/codegen_cases_assign.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment without &amp;" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="26">
   <si>
     <t>LHS Type</t>
   </si>
@@ -84,6 +84,15 @@
   </si>
   <si>
     <t>LEA (RHS.A), R | MOV R, (LHS.A)</t>
+  </si>
+  <si>
+    <t>MOV (RHS.A), R | MOV R, (LHS.A)</t>
+  </si>
+  <si>
+    <t>MOV (RHS.R), R | MOV R, (LHS.A)</t>
+  </si>
+  <si>
+    <t>MOV (RHS.A), R | MOV R, (LHS.R)</t>
   </si>
 </sst>
 </file>
@@ -450,7 +459,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -528,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1">
@@ -681,7 +690,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1">
@@ -800,7 +809,7 @@
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1">
@@ -953,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1">
@@ -1054,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>